<commit_message>
add music and update tetris fb
</commit_message>
<xml_diff>
--- a/Pic/listani.xlsx
+++ b/Pic/listani.xlsx
@@ -559,8 +559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
add images and vi
</commit_message>
<xml_diff>
--- a/Pic/listani.xlsx
+++ b/Pic/listani.xlsx
@@ -51,9 +51,6 @@
     <t>CON CHÓ - dog</t>
   </si>
   <si>
-    <t>CON  SÓI - wolf</t>
-  </si>
-  <si>
     <t>CON CHUỒN CHUỒN - Dragonfly</t>
   </si>
   <si>
@@ -126,9 +123,6 @@
     <t>CON KIẾN - ant</t>
   </si>
   <si>
-    <t>CON GẤU KOALA - koala</t>
-  </si>
-  <si>
     <t>CON LẠC ĐÀ - camel</t>
   </si>
   <si>
@@ -171,9 +165,6 @@
     <t>CON SAO BIỂN - Starfish</t>
   </si>
   <si>
-    <t>CON Giun- worm</t>
-  </si>
-  <si>
     <t>CON SÓC - SQUIRREL</t>
   </si>
   <si>
@@ -226,6 +217,15 @@
   </si>
   <si>
     <t>CON THẰN LẰN - house gecko</t>
+  </si>
+  <si>
+    <t>CON sâu- worm</t>
+  </si>
+  <si>
+    <t>CON  chó SÓI - wolf</t>
+  </si>
+  <si>
+    <t>CON GẤU trúc - koala</t>
   </si>
 </sst>
 </file>
@@ -559,7 +559,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
       <selection activeCell="A70" sqref="A70"/>
     </sheetView>
   </sheetViews>
@@ -625,297 +625,297 @@
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="s">
-        <v>36</v>
+        <v>69</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>